<commit_message>
[Billing] edit excel template
</commit_message>
<xml_diff>
--- a/src/main/resources/forms/invoice_excel.xlsx
+++ b/src/main/resources/forms/invoice_excel.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim Tung\IdeaProjects\support-server\src\main\resources\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimtung/IdeaProjects/support/src/main/resources/forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32000" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,23 +29,23 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Microsoft Office User</author>
     <author>Kim Tung</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <rFont val="Calibri"/>
           </rPr>
-          <t>jx:area(lastCell="G4")</t>
+          <t>jx:area(lastCell="G9")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A8" authorId="1">
       <text>
         <r>
           <rPr>
@@ -50,9 +53,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="invoices" var="invoice" lastCell="G4")
+          <t xml:space="preserve">jx:each(items="invoices" var="invoice" lastCell="G8")
 </t>
         </r>
       </text>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Invoice ID</t>
   </si>
@@ -101,13 +103,31 @@
   </si>
   <si>
     <t>${invoice.feePerUser}</t>
+  </si>
+  <si>
+    <t>Summary:</t>
+  </si>
+  <si>
+    <t>INVOICES</t>
+  </si>
+  <si>
+    <t>Company ID:</t>
+  </si>
+  <si>
+    <t>Period:</t>
+  </si>
+  <si>
+    <t>${companyId}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,28 +136,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -145,12 +183,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,71 +617,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="13" t="str">
+        <f>TEXT(MIN(B8),"mmmm dd, yyyy") &amp; " - " &amp; TEXT(MAX(B8), "mmmm dd, yyyy")</f>
+        <v>January 00, 1900 - January 00, 1900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G7" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="8" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
+      <c r="G8" s="4" t="e">
+        <f xml:space="preserve"> E8 * F8</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="10" t="e">
+        <f>SUM(G8)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:G5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>